<commit_message>
Add ANOVA test and Post-hoc analysis
</commit_message>
<xml_diff>
--- a/data/휴인미 game result 복사본.xlsx
+++ b/data/휴인미 game result 복사본.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuns\H\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1CC5BB-D7B3-457E-8FE4-66C522D7514C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE93BC9C-0C53-4F68-8988-81F65B1429BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{91E208FB-A9F6-4555-BCA0-7AB9BCF5817E}"/>
   </bookViews>
@@ -1325,9 +1325,6 @@
     <t>47522</t>
   </si>
   <si>
-    <t>13,16,14,5,10,6,4,7,9,12,3,8,2,15,1,11</t>
-  </si>
-  <si>
     <t>2024-12-01 23:59:03.414222</t>
   </si>
   <si>
@@ -2508,6 +2505,10 @@
   </si>
   <si>
     <t>ظ,ت,ف,ث,ر,ج,ا,ل,م,ك,ب,د,ن,ص,ق,ط,خ,س,غ,ض,ش,ز,ع,ذ,ح</t>
+  </si>
+  <si>
+    <t>SHAPE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2531,12 +2532,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -2568,7 +2581,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2577,6 +2590,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2914,8 +2939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76CAF321-7E60-48D9-8975-E1A97ACB2B4E}">
   <dimension ref="A1:H217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H149" sqref="H149"/>
+    <sheetView tabSelected="1" topLeftCell="A136" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D148" sqref="D148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -2933,28 +2958,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.6">
       <c r="A1" s="2" t="s">
+        <v>686</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>687</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>688</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>689</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>690</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>691</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>692</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>693</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.6">
@@ -2971,13 +2996,13 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>694</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>695</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>696</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>697</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>1</v>
@@ -2997,13 +3022,13 @@
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>697</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>698</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>699</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>700</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>66</v>
@@ -3023,16 +3048,16 @@
         <v>6</v>
       </c>
       <c r="E4" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>701</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>702</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>703</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.6">
@@ -3049,42 +3074,42 @@
         <v>0</v>
       </c>
       <c r="E5" s="2" t="s">
+        <v>704</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>705</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>706</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A6" s="3">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3">
+        <v>16</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>707</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A6" s="2">
-        <v>1</v>
-      </c>
-      <c r="B6" s="2">
-        <v>16</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="3" t="s">
         <v>708</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="3" t="s">
         <v>709</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="3" t="s">
         <v>710</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>711</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.6">
@@ -3101,13 +3126,13 @@
         <v>0</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>711</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>712</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>713</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>714</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>70</v>
@@ -3127,16 +3152,16 @@
         <v>9</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>714</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>715</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>716</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>717</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>718</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.6">
@@ -3153,16 +3178,16 @@
         <v>8</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>718</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>719</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>720</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>721</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>722</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.6">
@@ -3179,16 +3204,16 @@
         <v>17</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>722</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>723</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>724</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>725</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>726</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.6">
@@ -3205,16 +3230,16 @@
         <v>7</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>726</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>727</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>728</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>729</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.6">
@@ -3231,16 +3256,16 @@
         <v>21</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>730</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>731</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>732</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>733</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>734</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.6">
@@ -3257,16 +3282,16 @@
         <v>16</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>734</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>735</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>736</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>737</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>738</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.6">
@@ -3283,13 +3308,13 @@
         <v>0</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>738</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>739</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>740</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>741</v>
       </c>
       <c r="H14" s="2" t="s">
         <v>1</v>
@@ -3309,13 +3334,13 @@
         <v>0</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>741</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>742</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>743</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>744</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>66</v>
@@ -3335,13 +3360,13 @@
         <v>0</v>
       </c>
       <c r="E16" s="2" t="s">
+        <v>744</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>745</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>746</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>747</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>110</v>
@@ -3361,42 +3386,42 @@
         <v>5</v>
       </c>
       <c r="E17" s="2" t="s">
+        <v>747</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>748</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>749</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="H17" s="2" t="s">
         <v>750</v>
       </c>
-      <c r="H17" s="2" t="s">
+    </row>
+    <row r="18" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A18" s="3">
+        <v>2</v>
+      </c>
+      <c r="B18" s="3">
+        <v>16</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>11</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>751</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A18" s="2">
-        <v>2</v>
-      </c>
-      <c r="B18" s="2">
-        <v>16</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D18" s="2">
-        <v>11</v>
-      </c>
-      <c r="E18" s="2" t="s">
+      <c r="F18" s="3" t="s">
         <v>752</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="G18" s="3" t="s">
         <v>753</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="H18" s="3" t="s">
         <v>754</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>755</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.6">
@@ -3413,13 +3438,13 @@
         <v>0</v>
       </c>
       <c r="E19" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>756</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>757</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>758</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>70</v>
@@ -3439,16 +3464,16 @@
         <v>7</v>
       </c>
       <c r="E20" s="2" t="s">
+        <v>758</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>759</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="G20" s="2" t="s">
         <v>760</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="H20" s="2" t="s">
         <v>761</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>762</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.6">
@@ -3465,16 +3490,16 @@
         <v>10</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>762</v>
+      </c>
+      <c r="F21" s="2" t="s">
         <v>763</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>764</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="H21" s="2" t="s">
         <v>765</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.6">
@@ -3491,16 +3516,16 @@
         <v>18</v>
       </c>
       <c r="E22" s="2" t="s">
+        <v>766</v>
+      </c>
+      <c r="F22" s="2" t="s">
         <v>767</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>768</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>769</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>770</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.6">
@@ -3517,13 +3542,13 @@
         <v>0</v>
       </c>
       <c r="E23" s="2" t="s">
+        <v>770</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>771</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>772</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>773</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>262</v>
@@ -3543,16 +3568,16 @@
         <v>19</v>
       </c>
       <c r="E24" s="2" t="s">
+        <v>773</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>774</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="G24" s="2" t="s">
         <v>775</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="H24" s="2" t="s">
         <v>776</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>777</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.6">
@@ -3569,16 +3594,16 @@
         <v>17</v>
       </c>
       <c r="E25" s="2" t="s">
+        <v>777</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>778</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="G25" s="2" t="s">
         <v>779</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="H25" s="2" t="s">
         <v>780</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>781</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.6">
@@ -3595,13 +3620,13 @@
         <v>0</v>
       </c>
       <c r="E26" s="2" t="s">
+        <v>781</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>782</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="G26" s="2" t="s">
         <v>783</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>784</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>1</v>
@@ -3621,13 +3646,13 @@
         <v>0</v>
       </c>
       <c r="E27" s="2" t="s">
+        <v>784</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>785</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="G27" s="2" t="s">
         <v>786</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>787</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>66</v>
@@ -3647,13 +3672,13 @@
         <v>0</v>
       </c>
       <c r="E28" s="2" t="s">
+        <v>787</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>788</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="G28" s="2" t="s">
         <v>789</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>790</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>110</v>
@@ -3673,42 +3698,42 @@
         <v>0</v>
       </c>
       <c r="E29" s="2" t="s">
+        <v>790</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>791</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="G29" s="2" t="s">
         <v>792</v>
       </c>
-      <c r="G29" s="2" t="s">
+      <c r="H29" s="2" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A30" s="3">
+        <v>3</v>
+      </c>
+      <c r="B30" s="3">
+        <v>16</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D30" s="3">
+        <v>4</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>793</v>
       </c>
-      <c r="H29" s="2" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A30" s="2">
-        <v>3</v>
-      </c>
-      <c r="B30" s="2">
-        <v>16</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D30" s="2">
-        <v>4</v>
-      </c>
-      <c r="E30" s="2" t="s">
+      <c r="F30" s="3" t="s">
         <v>794</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="G30" s="3" t="s">
         <v>795</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="H30" s="3" t="s">
         <v>796</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>797</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.6">
@@ -3725,13 +3750,13 @@
         <v>0</v>
       </c>
       <c r="E31" s="2" t="s">
+        <v>797</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>798</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="G31" s="2" t="s">
         <v>799</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>800</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>70</v>
@@ -3751,16 +3776,16 @@
         <v>4</v>
       </c>
       <c r="E32" s="2" t="s">
+        <v>800</v>
+      </c>
+      <c r="F32" s="2" t="s">
         <v>801</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="G32" s="2" t="s">
         <v>802</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="H32" s="2" t="s">
         <v>803</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>804</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.6">
@@ -3777,16 +3802,16 @@
         <v>5</v>
       </c>
       <c r="E33" s="2" t="s">
+        <v>804</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>805</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="G33" s="2" t="s">
         <v>806</v>
       </c>
-      <c r="G33" s="2" t="s">
+      <c r="H33" s="2" t="s">
         <v>807</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>808</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.6">
@@ -3803,16 +3828,16 @@
         <v>12</v>
       </c>
       <c r="E34" s="2" t="s">
+        <v>808</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>809</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="G34" s="2" t="s">
         <v>810</v>
       </c>
-      <c r="G34" s="2" t="s">
+      <c r="H34" s="2" t="s">
         <v>811</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>812</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.6">
@@ -3829,13 +3854,13 @@
         <v>0</v>
       </c>
       <c r="E35" s="2" t="s">
+        <v>812</v>
+      </c>
+      <c r="F35" s="2" t="s">
         <v>813</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="G35" s="2" t="s">
         <v>814</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>815</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>262</v>
@@ -3855,16 +3880,16 @@
         <v>8</v>
       </c>
       <c r="E36" s="2" t="s">
+        <v>815</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>816</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="G36" s="2" t="s">
         <v>817</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="H36" s="2" t="s">
         <v>818</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>819</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.6">
@@ -3881,16 +3906,16 @@
         <v>14</v>
       </c>
       <c r="E37" s="2" t="s">
+        <v>819</v>
+      </c>
+      <c r="F37" s="2" t="s">
         <v>820</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="G37" s="2" t="s">
         <v>821</v>
       </c>
-      <c r="G37" s="2" t="s">
+      <c r="H37" s="2" t="s">
         <v>822</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>823</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.6">
@@ -3997,29 +4022,29 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A42" s="2">
+    <row r="42" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A42" s="3">
         <v>4</v>
       </c>
-      <c r="B42" s="2">
-        <v>16</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D42" s="2">
+      <c r="B42" s="3">
+        <v>16</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="3">
         <v>11</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="E42" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="F42" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G42" s="2" t="s">
+      <c r="G42" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H42" s="2" t="s">
+      <c r="H42" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -4231,29 +4256,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A51" s="2">
+    <row r="51" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A51" s="3">
         <v>5</v>
       </c>
-      <c r="B51" s="2">
-        <v>16</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D51" s="2">
-        <v>9</v>
-      </c>
-      <c r="E51" s="2" t="s">
+      <c r="B51" s="3">
+        <v>16</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D51" s="3">
+        <v>9</v>
+      </c>
+      <c r="E51" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="F51" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="G51" s="2" t="s">
+      <c r="G51" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="H51" s="2" t="s">
+      <c r="H51" s="3" t="s">
         <v>58</v>
       </c>
     </row>
@@ -4621,29 +4646,29 @@
         <v>114</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A66" s="2">
+    <row r="66" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A66" s="3">
         <v>6</v>
       </c>
-      <c r="B66" s="2">
-        <v>16</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D66" s="2">
+      <c r="B66" s="3">
+        <v>16</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D66" s="3">
         <v>14</v>
       </c>
-      <c r="E66" s="2" t="s">
+      <c r="E66" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="F66" s="2" t="s">
+      <c r="F66" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="G66" s="2" t="s">
+      <c r="G66" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="H66" s="2" t="s">
+      <c r="H66" s="3" t="s">
         <v>118</v>
       </c>
     </row>
@@ -4933,29 +4958,29 @@
         <v>160</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A78" s="2">
+    <row r="78" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A78" s="3">
         <v>7</v>
       </c>
-      <c r="B78" s="2">
-        <v>16</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D78" s="2">
+      <c r="B78" s="3">
+        <v>16</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D78" s="3">
         <v>11</v>
       </c>
-      <c r="E78" s="2" t="s">
+      <c r="E78" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="F78" s="2" t="s">
+      <c r="F78" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="G78" s="2" t="s">
+      <c r="G78" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="H78" s="2" t="s">
+      <c r="H78" s="3" t="s">
         <v>164</v>
       </c>
     </row>
@@ -5167,29 +5192,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A87" s="2">
+    <row r="87" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A87" s="3">
         <v>8</v>
       </c>
-      <c r="B87" s="2">
-        <v>16</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D87" s="2">
+      <c r="B87" s="3">
+        <v>16</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D87" s="3">
         <v>11</v>
       </c>
-      <c r="E87" s="2" t="s">
+      <c r="E87" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="F87" s="2" t="s">
+      <c r="F87" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="G87" s="2" t="s">
+      <c r="G87" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="H87" s="2" t="s">
+      <c r="H87" s="3" t="s">
         <v>200</v>
       </c>
     </row>
@@ -5479,29 +5504,29 @@
         <v>242</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A99" s="2">
-        <v>9</v>
-      </c>
-      <c r="B99" s="2">
-        <v>16</v>
-      </c>
-      <c r="C99" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D99" s="2">
+    <row r="99" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A99" s="3">
+        <v>9</v>
+      </c>
+      <c r="B99" s="3">
+        <v>16</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D99" s="3">
         <v>4</v>
       </c>
-      <c r="E99" s="2" t="s">
+      <c r="E99" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="F99" s="2" t="s">
+      <c r="F99" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="G99" s="2" t="s">
+      <c r="G99" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="H99" s="2" t="s">
+      <c r="H99" s="3" t="s">
         <v>246</v>
       </c>
     </row>
@@ -5869,29 +5894,29 @@
         <v>230</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A114" s="2">
+    <row r="114" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A114" s="3">
         <v>10</v>
       </c>
-      <c r="B114" s="2">
-        <v>16</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D114" s="2">
+      <c r="B114" s="3">
+        <v>16</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D114" s="3">
         <v>8</v>
       </c>
-      <c r="E114" s="2" t="s">
+      <c r="E114" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="F114" s="2" t="s">
+      <c r="F114" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="G114" s="2" t="s">
+      <c r="G114" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="H114" s="2" t="s">
+      <c r="H114" s="3" t="s">
         <v>302</v>
       </c>
     </row>
@@ -6181,29 +6206,29 @@
         <v>344</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A126" s="2">
+    <row r="126" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A126" s="3">
         <v>11</v>
       </c>
-      <c r="B126" s="2">
-        <v>16</v>
-      </c>
-      <c r="C126" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D126" s="2">
+      <c r="B126" s="3">
+        <v>16</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D126" s="3">
         <v>12</v>
       </c>
-      <c r="E126" s="2" t="s">
+      <c r="E126" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="F126" s="2" t="s">
+      <c r="F126" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="G126" s="2" t="s">
+      <c r="G126" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="H126" s="2" t="s">
+      <c r="H126" s="3" t="s">
         <v>348</v>
       </c>
     </row>
@@ -6415,29 +6440,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A135" s="2">
+    <row r="135" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A135" s="3">
         <v>12</v>
       </c>
-      <c r="B135" s="2">
-        <v>16</v>
-      </c>
-      <c r="C135" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D135" s="2">
+      <c r="B135" s="3">
+        <v>16</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D135" s="3">
         <v>8</v>
       </c>
-      <c r="E135" s="2" t="s">
+      <c r="E135" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="F135" s="2" t="s">
+      <c r="F135" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="G135" s="2" t="s">
+      <c r="G135" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="H135" s="2" t="s">
+      <c r="H135" s="3" t="s">
         <v>383</v>
       </c>
     </row>
@@ -6663,7 +6688,7 @@
         <v>15</v>
       </c>
       <c r="E144" s="2" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="F144" s="2" t="s">
         <v>416</v>
@@ -6692,7 +6717,7 @@
         <v>415</v>
       </c>
       <c r="F145" s="2" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G145" s="2" t="s">
         <v>417</v>
@@ -6718,7 +6743,7 @@
         <v>419</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G146" s="2" t="s">
         <v>421</v>
@@ -6744,7 +6769,7 @@
         <v>423</v>
       </c>
       <c r="F147" s="2" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G147" s="2" t="s">
         <v>425</v>
@@ -6753,30 +6778,30 @@
         <v>66</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A148" s="2">
+    <row r="148" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A148" s="5">
         <v>13</v>
       </c>
-      <c r="B148" s="2">
-        <v>16</v>
-      </c>
-      <c r="C148" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D148" s="2">
-        <v>2</v>
-      </c>
-      <c r="E148" s="2" t="s">
+      <c r="B148" s="5">
+        <v>9</v>
+      </c>
+      <c r="C148" s="5" t="s">
+        <v>823</v>
+      </c>
+      <c r="D148" s="5">
+        <v>2</v>
+      </c>
+      <c r="E148" s="5" t="s">
         <v>426</v>
       </c>
-      <c r="F148" s="2" t="s">
+      <c r="F148" s="5" t="s">
         <v>420</v>
       </c>
-      <c r="G148" s="2" t="s">
+      <c r="G148" s="5" t="s">
         <v>428</v>
       </c>
-      <c r="H148" s="2" t="s">
-        <v>429</v>
+      <c r="H148" s="5" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.6">
@@ -6793,16 +6818,16 @@
         <v>3</v>
       </c>
       <c r="E149" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F149" s="2" t="s">
         <v>424</v>
       </c>
       <c r="G149" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="H149" s="2" t="s">
         <v>432</v>
-      </c>
-      <c r="H149" s="2" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.6">
@@ -6819,41 +6844,41 @@
         <v>0</v>
       </c>
       <c r="E150" s="2" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F150" s="2" t="s">
         <v>427</v>
       </c>
       <c r="G150" s="2" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H150" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A151" s="2">
+    <row r="151" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A151" s="3">
         <v>13</v>
       </c>
-      <c r="B151" s="2">
-        <v>16</v>
-      </c>
-      <c r="C151" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D151" s="2">
-        <v>0</v>
-      </c>
-      <c r="E151" s="2" t="s">
-        <v>437</v>
-      </c>
-      <c r="F151" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="G151" s="2" t="s">
-        <v>439</v>
-      </c>
-      <c r="H151" s="2" t="s">
+      <c r="B151" s="3">
+        <v>16</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D151" s="3">
+        <v>0</v>
+      </c>
+      <c r="E151" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="F151" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="G151" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="H151" s="3" t="s">
         <v>193</v>
       </c>
     </row>
@@ -6871,16 +6896,16 @@
         <v>9</v>
       </c>
       <c r="E152" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F152" s="2" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="G152" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="H152" s="2" t="s">
         <v>442</v>
-      </c>
-      <c r="H152" s="2" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.6">
@@ -6897,16 +6922,16 @@
         <v>4</v>
       </c>
       <c r="E153" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="F153" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="G153" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="H153" s="2" t="s">
         <v>446</v>
-      </c>
-      <c r="H153" s="2" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.6">
@@ -6923,16 +6948,16 @@
         <v>5</v>
       </c>
       <c r="E154" s="2" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F154" s="2" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="G154" s="2" t="s">
+        <v>449</v>
+      </c>
+      <c r="H154" s="2" t="s">
         <v>450</v>
-      </c>
-      <c r="H154" s="2" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.6">
@@ -6949,16 +6974,16 @@
         <v>11</v>
       </c>
       <c r="E155" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="F155" s="2" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="G155" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="H155" s="2" t="s">
         <v>454</v>
-      </c>
-      <c r="H155" s="2" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.6">
@@ -6975,16 +7000,16 @@
         <v>5</v>
       </c>
       <c r="E156" s="2" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="F156" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="G156" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="H156" s="2" t="s">
         <v>458</v>
-      </c>
-      <c r="H156" s="2" t="s">
-        <v>459</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.6">
@@ -7001,16 +7026,16 @@
         <v>23</v>
       </c>
       <c r="E157" s="2" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F157" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="G157" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="H157" s="2" t="s">
         <v>462</v>
-      </c>
-      <c r="H157" s="2" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.6">
@@ -7027,13 +7052,13 @@
         <v>0</v>
       </c>
       <c r="E158" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="F158" s="2" t="s">
         <v>464</v>
       </c>
-      <c r="F158" s="2" t="s">
+      <c r="G158" s="2" t="s">
         <v>465</v>
-      </c>
-      <c r="G158" s="2" t="s">
-        <v>466</v>
       </c>
       <c r="H158" s="2" t="s">
         <v>1</v>
@@ -7053,13 +7078,13 @@
         <v>0</v>
       </c>
       <c r="E159" s="2" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F159" s="2" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="G159" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="H159" s="2" t="s">
         <v>66</v>
@@ -7079,13 +7104,13 @@
         <v>0</v>
       </c>
       <c r="E160" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="F160" s="2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="G160" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="H160" s="2" t="s">
         <v>110</v>
@@ -7105,42 +7130,42 @@
         <v>6</v>
       </c>
       <c r="E161" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="F161" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="G161" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="H161" s="2" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A162" s="3">
+        <v>14</v>
+      </c>
+      <c r="B162" s="3">
+        <v>16</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D162" s="3">
+        <v>5</v>
+      </c>
+      <c r="E162" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="F162" s="3" t="s">
         <v>473</v>
       </c>
-      <c r="F161" s="2" t="s">
-        <v>471</v>
-      </c>
-      <c r="G161" s="2" t="s">
-        <v>475</v>
-      </c>
-      <c r="H161" s="2" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A162" s="2">
-        <v>14</v>
-      </c>
-      <c r="B162" s="2">
-        <v>16</v>
-      </c>
-      <c r="C162" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D162" s="2">
-        <v>5</v>
-      </c>
-      <c r="E162" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="F162" s="2" t="s">
-        <v>474</v>
-      </c>
-      <c r="G162" s="2" t="s">
+      <c r="G162" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="H162" s="3" t="s">
         <v>479</v>
-      </c>
-      <c r="H162" s="2" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.6">
@@ -7157,13 +7182,13 @@
         <v>0</v>
       </c>
       <c r="E163" s="2" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="F163" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="G163" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="H163" s="2" t="s">
         <v>70</v>
@@ -7183,16 +7208,16 @@
         <v>3</v>
       </c>
       <c r="E164" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F164" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="G164" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="H164" s="2" t="s">
         <v>486</v>
-      </c>
-      <c r="H164" s="2" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.6">
@@ -7209,16 +7234,16 @@
         <v>11</v>
       </c>
       <c r="E165" s="2" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F165" s="2" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="G165" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="H165" s="2" t="s">
         <v>490</v>
-      </c>
-      <c r="H165" s="2" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.6">
@@ -7235,16 +7260,16 @@
         <v>7</v>
       </c>
       <c r="E166" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F166" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="G166" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="H166" s="2" t="s">
         <v>494</v>
-      </c>
-      <c r="H166" s="2" t="s">
-        <v>495</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.6">
@@ -7261,13 +7286,13 @@
         <v>0</v>
       </c>
       <c r="E167" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F167" s="2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="G167" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="H167" s="2" t="s">
         <v>262</v>
@@ -7287,16 +7312,16 @@
         <v>14</v>
       </c>
       <c r="E168" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F168" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="G168" s="2" t="s">
+        <v>500</v>
+      </c>
+      <c r="H168" s="2" t="s">
         <v>501</v>
-      </c>
-      <c r="H168" s="2" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.6">
@@ -7313,16 +7338,16 @@
         <v>12</v>
       </c>
       <c r="E169" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F169" s="2" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="G169" s="2" t="s">
+        <v>504</v>
+      </c>
+      <c r="H169" s="2" t="s">
         <v>505</v>
-      </c>
-      <c r="H169" s="2" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.6">
@@ -7339,13 +7364,13 @@
         <v>0</v>
       </c>
       <c r="E170" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F170" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="G170" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="H170" s="2" t="s">
         <v>1</v>
@@ -7365,13 +7390,13 @@
         <v>0</v>
       </c>
       <c r="E171" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F171" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="G171" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H171" s="2" t="s">
         <v>66</v>
@@ -7391,16 +7416,16 @@
         <v>2</v>
       </c>
       <c r="E172" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F172" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="G172" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="H172" s="2" t="s">
         <v>515</v>
-      </c>
-      <c r="H172" s="2" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.6">
@@ -7417,42 +7442,42 @@
         <v>5</v>
       </c>
       <c r="E173" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F173" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="G173" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="H173" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="H173" s="2" t="s">
+    </row>
+    <row r="174" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A174" s="3">
+        <v>15</v>
+      </c>
+      <c r="B174" s="3">
+        <v>16</v>
+      </c>
+      <c r="C174" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D174" s="3">
+        <v>11</v>
+      </c>
+      <c r="E174" s="3" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A174" s="2">
-        <v>15</v>
-      </c>
-      <c r="B174" s="2">
-        <v>16</v>
-      </c>
-      <c r="C174" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D174" s="2">
-        <v>11</v>
-      </c>
-      <c r="E174" s="2" t="s">
-        <v>521</v>
-      </c>
-      <c r="F174" s="2" t="s">
-        <v>504</v>
-      </c>
-      <c r="G174" s="2" t="s">
+      <c r="F174" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="G174" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="H174" s="3" t="s">
         <v>523</v>
-      </c>
-      <c r="H174" s="2" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.6">
@@ -7469,13 +7494,13 @@
         <v>0</v>
       </c>
       <c r="E175" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="F175" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G175" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="H175" s="2" t="s">
         <v>70</v>
@@ -7495,16 +7520,16 @@
         <v>8</v>
       </c>
       <c r="E176" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F176" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G176" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="H176" s="2" t="s">
         <v>530</v>
-      </c>
-      <c r="H176" s="2" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.6">
@@ -7521,16 +7546,16 @@
         <v>14</v>
       </c>
       <c r="E177" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="F177" s="2" t="s">
+        <v>513</v>
+      </c>
+      <c r="G177" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="F177" s="2" t="s">
-        <v>514</v>
-      </c>
-      <c r="G177" s="2" t="s">
+      <c r="H177" s="2" t="s">
         <v>533</v>
-      </c>
-      <c r="H177" s="2" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.6">
@@ -7547,16 +7572,16 @@
         <v>20</v>
       </c>
       <c r="E178" s="2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F178" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G178" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="H178" s="2" t="s">
         <v>537</v>
-      </c>
-      <c r="H178" s="2" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.6">
@@ -7573,16 +7598,16 @@
         <v>2</v>
       </c>
       <c r="E179" s="2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F179" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="G179" s="2" t="s">
+        <v>540</v>
+      </c>
+      <c r="H179" s="2" t="s">
         <v>541</v>
-      </c>
-      <c r="H179" s="2" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.6">
@@ -7599,16 +7624,16 @@
         <v>22</v>
       </c>
       <c r="E180" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="F180" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="G180" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="H180" s="2" t="s">
         <v>545</v>
-      </c>
-      <c r="H180" s="2" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.6">
@@ -7625,16 +7650,16 @@
         <v>23</v>
       </c>
       <c r="E181" s="2" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F181" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="G181" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="H181" s="2" t="s">
         <v>549</v>
-      </c>
-      <c r="H181" s="2" t="s">
-        <v>550</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.6">
@@ -7651,16 +7676,16 @@
         <v>3</v>
       </c>
       <c r="E182" s="2" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="F182" s="2" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="G182" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="H182" s="2" t="s">
         <v>555</v>
-      </c>
-      <c r="H182" s="2" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.6">
@@ -7677,13 +7702,13 @@
         <v>0</v>
       </c>
       <c r="E183" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F183" s="2" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G183" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="H183" s="2" t="s">
         <v>66</v>
@@ -7703,13 +7728,13 @@
         <v>0</v>
       </c>
       <c r="E184" s="2" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F184" s="2" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="G184" s="2" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="H184" s="2" t="s">
         <v>110</v>
@@ -7729,42 +7754,42 @@
         <v>0</v>
       </c>
       <c r="E185" s="2" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F185" s="2" t="s">
+        <v>681</v>
+      </c>
+      <c r="G185" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="H185" s="2" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A186" s="3">
+        <v>16</v>
+      </c>
+      <c r="B186" s="3">
+        <v>16</v>
+      </c>
+      <c r="C186" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D186" s="3">
+        <v>11</v>
+      </c>
+      <c r="E186" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="F186" s="3" t="s">
         <v>682</v>
       </c>
-      <c r="G185" s="2" t="s">
-        <v>565</v>
-      </c>
-      <c r="H185" s="2" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A186" s="2">
-        <v>16</v>
-      </c>
-      <c r="B186" s="2">
-        <v>16</v>
-      </c>
-      <c r="C186" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D186" s="2">
-        <v>11</v>
-      </c>
-      <c r="E186" s="2" t="s">
-        <v>567</v>
-      </c>
-      <c r="F186" s="2" t="s">
-        <v>683</v>
-      </c>
-      <c r="G186" s="2" t="s">
+      <c r="G186" s="3" t="s">
+        <v>568</v>
+      </c>
+      <c r="H186" s="3" t="s">
         <v>569</v>
-      </c>
-      <c r="H186" s="2" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.6">
@@ -7781,13 +7806,13 @@
         <v>0</v>
       </c>
       <c r="E187" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F187" s="2" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="G187" s="2" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H187" s="2" t="s">
         <v>70</v>
@@ -7807,16 +7832,16 @@
         <v>7</v>
       </c>
       <c r="E188" s="2" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="F188" s="2" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="G188" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="H188" s="2" t="s">
         <v>576</v>
-      </c>
-      <c r="H188" s="2" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.6">
@@ -7833,16 +7858,16 @@
         <v>14</v>
       </c>
       <c r="E189" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F189" s="2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="G189" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="H189" s="2" t="s">
         <v>580</v>
-      </c>
-      <c r="H189" s="2" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.6">
@@ -7859,16 +7884,16 @@
         <v>17</v>
       </c>
       <c r="E190" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F190" s="2" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="G190" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="H190" s="2" t="s">
         <v>584</v>
-      </c>
-      <c r="H190" s="2" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.6">
@@ -7885,16 +7910,16 @@
         <v>18</v>
       </c>
       <c r="E191" s="2" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F191" s="2" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="G191" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="H191" s="2" t="s">
         <v>588</v>
-      </c>
-      <c r="H191" s="2" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.6">
@@ -7911,16 +7936,16 @@
         <v>18</v>
       </c>
       <c r="E192" s="2" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="F192" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="G192" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="H192" s="2" t="s">
         <v>592</v>
-      </c>
-      <c r="H192" s="2" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.6">
@@ -7937,16 +7962,16 @@
         <v>15</v>
       </c>
       <c r="E193" s="2" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="F193" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="G193" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="H193" s="2" t="s">
         <v>596</v>
-      </c>
-      <c r="H193" s="2" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.6">
@@ -7963,13 +7988,13 @@
         <v>0</v>
       </c>
       <c r="E194" s="2" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="F194" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="G194" s="2" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="H194" s="2" t="s">
         <v>1</v>
@@ -7989,13 +8014,13 @@
         <v>0</v>
       </c>
       <c r="E195" s="2" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="F195" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="G195" s="2" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="H195" s="2" t="s">
         <v>66</v>
@@ -8015,13 +8040,13 @@
         <v>0</v>
       </c>
       <c r="E196" s="2" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F196" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="G196" s="2" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="H196" s="2" t="s">
         <v>110</v>
@@ -8041,42 +8066,42 @@
         <v>0</v>
       </c>
       <c r="E197" s="2" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="F197" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="G197" s="2" t="s">
+        <v>608</v>
+      </c>
+      <c r="H197" s="2" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A198" s="3">
+        <v>17</v>
+      </c>
+      <c r="B198" s="3">
+        <v>16</v>
+      </c>
+      <c r="C198" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D198" s="3">
+        <v>11</v>
+      </c>
+      <c r="E198" s="3" t="s">
         <v>609</v>
       </c>
-      <c r="H197" s="2" t="s">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A198" s="2">
-        <v>17</v>
-      </c>
-      <c r="B198" s="2">
-        <v>16</v>
-      </c>
-      <c r="C198" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D198" s="2">
-        <v>11</v>
-      </c>
-      <c r="E198" s="2" t="s">
-        <v>610</v>
-      </c>
-      <c r="F198" s="2" t="s">
-        <v>564</v>
-      </c>
-      <c r="G198" s="2" t="s">
+      <c r="F198" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="G198" s="3" t="s">
+        <v>611</v>
+      </c>
+      <c r="H198" s="3" t="s">
         <v>612</v>
-      </c>
-      <c r="H198" s="2" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.6">
@@ -8093,13 +8118,13 @@
         <v>0</v>
       </c>
       <c r="E199" s="2" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="F199" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="G199" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="H199" s="2" t="s">
         <v>70</v>
@@ -8119,16 +8144,16 @@
         <v>8</v>
       </c>
       <c r="E200" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="F200" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="G200" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="H200" s="2" t="s">
         <v>619</v>
-      </c>
-      <c r="H200" s="2" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.6">
@@ -8145,16 +8170,16 @@
         <v>10</v>
       </c>
       <c r="E201" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F201" s="2" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="G201" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="H201" s="2" t="s">
         <v>623</v>
-      </c>
-      <c r="H201" s="2" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.6">
@@ -8171,16 +8196,16 @@
         <v>19</v>
       </c>
       <c r="E202" s="2" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="F202" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="G202" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="H202" s="2" t="s">
         <v>627</v>
-      </c>
-      <c r="H202" s="2" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.6">
@@ -8197,16 +8222,16 @@
         <v>12</v>
       </c>
       <c r="E203" s="2" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="F203" s="2" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="G203" s="2" t="s">
+        <v>630</v>
+      </c>
+      <c r="H203" s="2" t="s">
         <v>631</v>
-      </c>
-      <c r="H203" s="2" t="s">
-        <v>632</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.6">
@@ -8223,16 +8248,16 @@
         <v>18</v>
       </c>
       <c r="E204" s="2" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F204" s="2" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G204" s="2" t="s">
+        <v>634</v>
+      </c>
+      <c r="H204" s="2" t="s">
         <v>635</v>
-      </c>
-      <c r="H204" s="2" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.6">
@@ -8249,16 +8274,16 @@
         <v>17</v>
       </c>
       <c r="E205" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="F205" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="G205" s="2" t="s">
         <v>637</v>
       </c>
-      <c r="F205" s="2" t="s">
-        <v>591</v>
-      </c>
-      <c r="G205" s="2" t="s">
+      <c r="H205" s="2" t="s">
         <v>638</v>
-      </c>
-      <c r="H205" s="2" t="s">
-        <v>639</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.6">
@@ -8275,13 +8300,13 @@
         <v>0</v>
       </c>
       <c r="E206" s="2" t="s">
+        <v>639</v>
+      </c>
+      <c r="F206" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="G206" s="2" t="s">
         <v>640</v>
-      </c>
-      <c r="F206" s="2" t="s">
-        <v>595</v>
-      </c>
-      <c r="G206" s="2" t="s">
-        <v>641</v>
       </c>
       <c r="H206" s="2" t="s">
         <v>1</v>
@@ -8301,16 +8326,16 @@
         <v>4</v>
       </c>
       <c r="E207" s="2" t="s">
+        <v>641</v>
+      </c>
+      <c r="F207" s="2" t="s">
+        <v>598</v>
+      </c>
+      <c r="G207" s="2" t="s">
         <v>642</v>
       </c>
-      <c r="F207" s="2" t="s">
-        <v>599</v>
-      </c>
-      <c r="G207" s="2" t="s">
+      <c r="H207" s="2" t="s">
         <v>643</v>
-      </c>
-      <c r="H207" s="2" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.6">
@@ -8327,13 +8352,13 @@
         <v>2</v>
       </c>
       <c r="E208" s="2" t="s">
+        <v>644</v>
+      </c>
+      <c r="F208" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="G208" s="2" t="s">
         <v>645</v>
-      </c>
-      <c r="F208" s="2" t="s">
-        <v>602</v>
-      </c>
-      <c r="G208" s="2" t="s">
-        <v>646</v>
       </c>
       <c r="H208" s="2" t="s">
         <v>218</v>
@@ -8353,42 +8378,42 @@
         <v>2</v>
       </c>
       <c r="E209" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="F209" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="G209" s="2" t="s">
         <v>647</v>
-      </c>
-      <c r="F209" s="2" t="s">
-        <v>605</v>
-      </c>
-      <c r="G209" s="2" t="s">
-        <v>648</v>
       </c>
       <c r="H209" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A210" s="2">
+    <row r="210" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="A210" s="3">
         <v>18</v>
       </c>
-      <c r="B210" s="2">
-        <v>16</v>
-      </c>
-      <c r="C210" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D210" s="2">
+      <c r="B210" s="3">
+        <v>16</v>
+      </c>
+      <c r="C210" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D210" s="3">
         <v>10</v>
       </c>
-      <c r="E210" s="2" t="s">
+      <c r="E210" s="3" t="s">
+        <v>648</v>
+      </c>
+      <c r="F210" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="G210" s="3" t="s">
         <v>649</v>
       </c>
-      <c r="F210" s="2" t="s">
-        <v>608</v>
-      </c>
-      <c r="G210" s="2" t="s">
+      <c r="H210" s="3" t="s">
         <v>650</v>
-      </c>
-      <c r="H210" s="2" t="s">
-        <v>651</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.6">
@@ -8405,16 +8430,16 @@
         <v>8</v>
       </c>
       <c r="E211" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="F211" s="2" t="s">
+        <v>610</v>
+      </c>
+      <c r="G211" s="2" t="s">
         <v>652</v>
       </c>
-      <c r="F211" s="2" t="s">
-        <v>611</v>
-      </c>
-      <c r="G211" s="2" t="s">
+      <c r="H211" s="2" t="s">
         <v>653</v>
-      </c>
-      <c r="H211" s="2" t="s">
-        <v>654</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.6">
@@ -8431,16 +8456,16 @@
         <v>10</v>
       </c>
       <c r="E212" s="2" t="s">
+        <v>654</v>
+      </c>
+      <c r="F212" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="G212" s="2" t="s">
         <v>655</v>
       </c>
-      <c r="F212" s="2" t="s">
-        <v>615</v>
-      </c>
-      <c r="G212" s="2" t="s">
+      <c r="H212" s="2" t="s">
         <v>656</v>
-      </c>
-      <c r="H212" s="2" t="s">
-        <v>657</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.6">
@@ -8457,16 +8482,16 @@
         <v>9</v>
       </c>
       <c r="E213" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="F213" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="G213" s="2" t="s">
         <v>658</v>
       </c>
-      <c r="F213" s="2" t="s">
-        <v>618</v>
-      </c>
-      <c r="G213" s="2" t="s">
+      <c r="H213" s="2" t="s">
         <v>659</v>
-      </c>
-      <c r="H213" s="2" t="s">
-        <v>660</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.6">
@@ -8483,16 +8508,16 @@
         <v>22</v>
       </c>
       <c r="E214" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="F214" s="2" t="s">
+        <v>621</v>
+      </c>
+      <c r="G214" s="2" t="s">
         <v>661</v>
       </c>
-      <c r="F214" s="2" t="s">
-        <v>622</v>
-      </c>
-      <c r="G214" s="2" t="s">
+      <c r="H214" s="2" t="s">
         <v>662</v>
-      </c>
-      <c r="H214" s="2" t="s">
-        <v>663</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.6">
@@ -8509,16 +8534,16 @@
         <v>5</v>
       </c>
       <c r="E215" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="F215" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="G215" s="2" t="s">
         <v>664</v>
       </c>
-      <c r="F215" s="2" t="s">
-        <v>626</v>
-      </c>
-      <c r="G215" s="2" t="s">
+      <c r="H215" s="2" t="s">
         <v>665</v>
-      </c>
-      <c r="H215" s="2" t="s">
-        <v>666</v>
       </c>
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.6">
@@ -8535,16 +8560,16 @@
         <v>18</v>
       </c>
       <c r="E216" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="F216" s="2" t="s">
+        <v>629</v>
+      </c>
+      <c r="G216" s="2" t="s">
         <v>667</v>
       </c>
-      <c r="F216" s="2" t="s">
-        <v>630</v>
-      </c>
-      <c r="G216" s="2" t="s">
+      <c r="H216" s="2" t="s">
         <v>668</v>
-      </c>
-      <c r="H216" s="2" t="s">
-        <v>669</v>
       </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.6">
@@ -8561,16 +8586,16 @@
         <v>20</v>
       </c>
       <c r="E217" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="F217" s="2" t="s">
+        <v>633</v>
+      </c>
+      <c r="G217" s="2" t="s">
         <v>670</v>
       </c>
-      <c r="F217" s="2" t="s">
-        <v>634</v>
-      </c>
-      <c r="G217" s="2" t="s">
+      <c r="H217" s="2" t="s">
         <v>671</v>
-      </c>
-      <c r="H217" s="2" t="s">
-        <v>672</v>
       </c>
     </row>
   </sheetData>

</xml_diff>